<commit_message>
Renamed action Removed unused function Cleaned up OR of unused objects Cleaned up OR names
</commit_message>
<xml_diff>
--- a/uft-one-ppm-ensure-logged-out/Default.xlsx
+++ b/uft-one-ppm-ensure-logged-out/Default.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="PPMProposalInitiation" sheetId="2" r:id="rId2"/>
+    <sheet name="PPMEnsureLoggedOut" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -181,9 +181,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -194,7 +192,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -536,10 +536,10 @@
       </c>
     </row>
     <row>
-      <c s="3" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>